<commit_message>
Updated Exam With Instructions Component
</commit_message>
<xml_diff>
--- a/public/datasets/rgn_7_fee.xlsx
+++ b/public/datasets/rgn_7_fee.xlsx
@@ -67,10 +67,10 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1732780206" val="1218" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1732780206" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1732780206" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1732780206"/>
+      <pm:revision xmlns:pm="smNativeData" day="1732787154" val="1218" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1732787154" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1732787154" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1732787154"/>
     </ext>
   </extLst>
 </workbook>
@@ -340,7 +340,7 @@
     <t>Aning Rhoda</t>
   </si>
   <si>
-    <t>PNMTC/DA/RGN/22/23/033l</t>
+    <t>PNMTC/DA/RGN/22/23/033</t>
   </si>
   <si>
     <t xml:space="preserve"> Agyemang Nketia G</t>
@@ -1425,7 +1425,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1732780206" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1732787154" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1440,7 +1440,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1732780206" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1732787154" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1455,7 +1455,7 @@
       <sz val="8"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1732780206" fgClr="323232" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1732787154" fgClr="323232" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="160" lang="default"/>
             <pm:cs face="Basic Roman" sz="160" lang="default"/>
             <pm:ea face="Basic Roman" sz="160" lang="default"/>
@@ -1470,7 +1470,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1732780206" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1732787154" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1492,7 +1492,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1732780206" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1732787154" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -1514,7 +1514,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1732780206"/>
+          <pm:border xmlns:pm="smNativeData" id="1732787154"/>
         </ext>
       </extLst>
     </border>
@@ -1533,7 +1533,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1732780206"/>
+          <pm:border xmlns:pm="smNativeData" id="1732787154"/>
         </ext>
       </extLst>
     </border>
@@ -1560,10 +1560,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1732780206" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1732787154" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1732780206" count="1">
+      <pm:colors xmlns:pm="smNativeData" id="1732787154" count="1">
         <pm:color name="Color 24" rgb="323232"/>
       </pm:colors>
     </ext>
@@ -1830,8 +1830,8 @@
   <dimension ref="A1:C219"/>
   <sheetViews>
     <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
+      <pane ySplit="2" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.40"/>
@@ -4254,7 +4254,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1732780206" printRowHead="0" printColHead="0" printHeadLine="1" printFootLine="1" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1732787154" printRowHead="0" printColHead="0" printHeadLine="1" printFootLine="1" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -4269,14 +4269,14 @@
     <oddFooter>&amp;R&amp;"Arial"&amp;8 Page &amp;P of &amp;N</oddFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1732780206" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1732780206" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1732787154" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1732787154" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1732780206" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1732787154" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>